<commit_message>
According to all known laws of aviation, there is no way that a bee should be able to fly. Its wings are too small to get its fat little body off the ground. The bee, of course, flies anyway because bees don't care what humans think is impossible
</commit_message>
<xml_diff>
--- a/Cleaned_Bangladesh_Food_Diary.xlsx
+++ b/Cleaned_Bangladesh_Food_Diary.xlsx
@@ -660,7 +660,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {1.95}; UNKNOWN; Small fish fry* {1.05}; UNKNOWN</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Small fish fry* {2.1}</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.65}; UNKNOWN; Hilsha, without bones, raw {0.35}</t>
+          <t>Rice, BR-28, boiled* (without salt) {6.0}; Hilsha, without bones, raw {1.0}</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Chicken leg, without skin, raw {0.35}; Potato, Diamond, boiled* (without salt) {0.16}; Ginger root, raw {0.1}; Onion, raw {0.16}; Chilli, green, with seeds, raw {0.16}; Coriander seed, dry {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {0.35}; Potato, Diamond, boiled* (without salt) {0.22}; Ginger root, raw {0.1}; Onion, raw {0.22}; Chilli, green, with seeds, raw {0.22}; Coriander seed, dry {0.1}</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -858,7 +858,7 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.26}; UNKNOWN; Beef, meat, lean, boneless, raw {0.7}; Potato, Diamond, boiled* (without salt) {0.26}; Ginger root, raw {0.1}; Onion, raw {0.26}; Garlic, raw {0.26}; Chilli, green, with seeds, raw {0.26}; Coriander seed, dry {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Beef, meat, lean, boneless, raw {0.7}; Potato, Diamond, boiled* (without salt) {0.33}; Ginger root, raw {0.1}; Onion, raw {0.33}; Garlic, raw {0.33}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.11}; UNKNOWN; Hilsha, without bones, raw {0.09}; Pangas, without bones, raw {0.09}; Potato, Diamond, boiled* (without salt) {0.11}; Tomato, red, ripe, boiled* (without salt) {0.11}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.09}; Pangas, without bones, raw {0.09}; Potato, Diamond, boiled* (without salt) {0.16}; Tomato, red, ripe, boiled* (without salt) {0.16}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Hilsha, without bones, raw {0.17}; Tilapia, without bones, raw {0.17}; Potato, Diamond, boiled* (without salt) {0.16}; Carrot, boiled* (without salt) {0.16}; Tomato, red, ripe, boiled* (without salt) {0.16}; Chilli, red, dry {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.17}; Tilapia, without bones, raw {0.17}; Potato, Diamond, boiled* (without salt) {0.22}; Carrot, boiled* (without salt) {0.22}; Tomato, red, ripe, boiled* (without salt) {0.22}; Chilli, red, dry {0.1}</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
@@ -968,7 +968,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.65}; UNKNOWN; Hilsha, without bones, raw {0.53}; Pangas, without bones, raw {0.53}; UNKNOWN; Carrot, boiled* (without salt) {0.65}; Brinjal, purple, long, boiled* (without salt) {0.65}</t>
+          <t>Rice, BR-28, boiled* (without salt) {6.0}; Hilsha, without bones, raw {0.53}; Pangas, without bones, raw {0.53}; UNKNOWN; Carrot, boiled* (without salt) {0.97}; Brinjal, purple, long, boiled* (without salt) {0.97}</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Chicken leg, without skin, raw {0.35}; Potato, Diamond, boiled* (without salt) {0.16}; Ginger root, raw {0.1}; Garlic, raw {0.16}; Chilli, green, with seeds, raw {0.16}; Coriander seed, dry {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {0.35}; Potato, Diamond, boiled* (without salt) {0.22}; Ginger root, raw {0.1}; Garlic, raw {0.22}; Chilli, green, with seeds, raw {0.22}; Coriander seed, dry {0.1}</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.11}; UNKNOWN; Hilsha, without bones, raw {0.09}; Pangas, without bones, raw {0.09}; Potato, Diamond, boiled* (without salt) {0.11}; Tomato, red, ripe, boiled* (without salt) {0.11}; Chilli, red, dry {0.1}; UNKNOWN</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.09}; Pangas, without bones, raw {0.09}; Potato, Diamond, boiled* (without salt) {0.16}; Tomato, red, ripe, boiled* (without salt) {0.16}; Chilli, red, dry {0.1}; UNKNOWN</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Beef, meat, lean, boneless, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.16}; Carrot, boiled* (without salt) {0.16}; Ginger root, raw {0.1}; Onion, raw {0.16}; Garlic, raw {0.16}; Chilli, green, with seeds, raw {0.16}; Coriander seed, dry {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Beef, meat, lean, boneless, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.2}; Carrot, boiled* (without salt) {0.2}; Ginger root, raw {0.1}; Onion, raw {0.2}; Garlic, raw {0.2}; Chilli, green, with seeds, raw {0.2}; Coriander seed, dry {0.1}</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Biscuit, sweet* {0.5}; Water, drinking {0.5}; UNKNOWN</t>
+          <t>Biscuit, sweet* {1.0}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Biscuit, sweet* {0.25}; Water, drinking {0.25}; UNKNOWN</t>
+          <t>Biscuit, sweet* {0.5}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {0.5}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.5}; Carrot, boiled* (without salt) {0.5}; Green gram, split, boiled* (without salt) {0.5}</t>
+          <t>Bread, bun/roll {0.5}; Potato, Diamond, boiled* (without salt) {0.67}; Carrot, boiled* (without salt) {0.67}; Green gram, split, boiled* (without salt) {0.67}</t>
         </is>
       </c>
       <c r="X5" t="inlineStr"/>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {0.67}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.67}; Green gram, split, boiled* (without salt) {0.67}</t>
+          <t>Bread, bun/roll {1.0}; Potato, Diamond, boiled* (without salt) {1.0}; Green gram, split, boiled* (without salt) {1.0}</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr"/>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {0.5}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.5}; Green gram, split, boiled* (without salt) {0.5}; Gourd, pointed, boiled* (without salt) {0.5}</t>
+          <t>Bread, bun/roll {0.5}; Potato, Diamond, boiled* (without salt) {0.67}; Green gram, split, boiled* (without salt) {0.67}; Gourd, pointed, boiled* (without salt) {0.67}</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr"/>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.11}; UNKNOWN; Egg, chicken, farmed, boiled* (without salt) {0.17}; Potato, Diamond, boiled* (without salt) {0.11}; Onion, raw {0.11}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {1.5}; Egg, chicken, farmed, boiled* (without salt) {0.17}; Potato, Diamond, boiled* (without salt) {0.16}; Onion, raw {0.16}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Hilsha, without bones, raw {0.7}; Turmeric, dried {0.1}; Soybean oil {0.15}; Potato, Diamond, boiled* (without salt) {0.33}; Cumin seeds {0.1}; Gourd, bitter, boiled* (without salt) {0.33}; Green gram, split, boiled* (without salt) {0.33}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.7}; Turmeric, dried {0.1}; Soybean oil {0.15}; Potato, Diamond, boiled* (without salt) {0.43}; Cumin seeds {0.1}; Gourd, bitter, boiled* (without salt) {0.43}; Green gram, split, boiled* (without salt) {0.43}</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Hilsha, without bones, raw {0.7}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.33}; Colocasia/Taro, boiled* (without salt) {0.33}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {1.0}; Potato, Diamond, boiled* (without salt) {0.67}; Colocasia/Taro, boiled* (without salt) {0.67}; Chilli, green, with seeds, raw {0.67}; Coriander seed, dry {0.1}</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.2}; UNKNOWN; Beef, meat, lean, boneless, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.2}; Carrot, boiled* (without salt) {0.2}; Chilli, green, with seeds, raw {0.2}; Coriander seed, dry {0.1}; Green gram, split, boiled* (without salt) {0.2}; UNKNOWN</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Beef, meat, lean, boneless, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.24}; Carrot, boiled* (without salt) {0.24}; Chilli, green, with seeds, raw {0.24}; Coriander seed, dry {0.1}; Green gram, split, boiled* (without salt) {0.24}; UNKNOWN</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {1.0}; UNKNOWN; Milk, cow, whole fat (pasteurized, UTH) {1.0}</t>
+          <t>Rice, BR-28, boiled* (without salt) {6.0}; Milk, cow, whole fat (pasteurized, UTH) {2.0}</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr"/>
@@ -1468,7 +1468,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.97}; UNKNOWN; Egg, chicken, farmed, boiled* (without salt) {1.05}; Onion, raw {0.97}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {1.05}; Onion, raw {1.95}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Beef, meat, lean, boneless, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.33}; Cumin seeds {0.1}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {6.0}; Beef, meat, lean, boneless, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.49}; Cumin seeds {0.1}; Chilli, green, with seeds, raw {0.49}; Coriander seed, dry {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Hilsha, without bones, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.33}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {6.0}; Hilsha, without bones, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.49}; Chilli, green, with seeds, raw {0.49}; Coriander seed, dry {0.1}</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Hilsha, without bones, raw {0.17}; Hilsha, without bones, raw {0.17}; Colocasia/Taro, boiled* (without salt) {0.33}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.17}; Hilsha, without bones, raw {0.17}; Colocasia/Taro, boiled* (without salt) {0.65}</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {0.8}; UNKNOWN; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.8}; Papaya, unripe, boiled* (without salt) {0.8}; Green gram, split, boiled* (without salt) {0.8}; Soybean oil {0.15}; Garlic, raw {0.8}</t>
+          <t>Bread, bun/roll {0.5}; Potato, Diamond, boiled* (without salt) {1.0}; Papaya, unripe, boiled* (without salt) {1.0}; Green gram, split, boiled* (without salt) {1.0}; Soybean oil {0.15}; Garlic, raw {1.0}</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Potato, Diamond, boiled* (without salt) {1.0}; Onion, raw {1.0}; Chilli, red, dry {0.1}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {1.0}</t>
+          <t>Bread, bun/roll {0.5}; Potato, Diamond, boiled* (without salt) {1.33}; Onion, raw {1.33}; Chilli, red, dry {0.1}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {1.33}</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
@@ -1686,7 +1686,7 @@
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.5}; UNKNOWN; Sugar, white {1.5}</t>
+          <t>Bread, bun/roll {1.0}; Sugar, white {3.0}</t>
         </is>
       </c>
       <c r="X8" t="inlineStr"/>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {0.21}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.21}; Carrot, boiled* (without salt) {0.21}; Cauliflower, boiled* (without salt) {0.21}; Cabbage, boiled* (without salt) {0.21}; Bean, seeds and pods, raw {0.21}; Brinjal, purple, long, boiled* (without salt) {0.21}; Chilli, red, dry {0.1}; Coriander leaves, raw {0.1}</t>
+          <t>Bread, bun/roll {0.5}; Potato, Diamond, boiled* (without salt) {0.25}; Carrot, boiled* (without salt) {0.25}; Cauliflower, boiled* (without salt) {0.25}; Cabbage, boiled* (without salt) {0.25}; Bean, seeds and pods, raw {0.25}; Brinjal, purple, long, boiled* (without salt) {0.25}; Chilli, red, dry {0.1}; Coriander leaves, raw {0.1}</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr"/>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {0.3}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.3}; Green gram, split, boiled* (without salt) {0.3}; Papaya, unripe, boiled* (without salt) {0.3}; Carrot, boiled* (without salt) {0.3}; Soybean oil {0.15}</t>
+          <t>Bread, bun/roll {1.0}; Potato, Diamond, boiled* (without salt) {0.38}; Green gram, split, boiled* (without salt) {0.38}; Papaya, unripe, boiled* (without salt) {0.38}; Carrot, boiled* (without salt) {0.38}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr"/>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Biscuit, sweet* {0.5}; UNKNOWN; Orange juice, raw (unsweetened) {0.5}; UNKNOWN</t>
+          <t>Biscuit, sweet* {0.75}; Orange juice, raw (unsweetened) {2.5}</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.08}; UNKNOWN; Hilsha, without bones, raw {0.09}; Hilsha, without bones, raw {0.09}; Gourd, pointed, boiled* (without salt) {0.08}; Onion, raw {0.08}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.08}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.09}; Hilsha, without bones, raw {0.09}; Gourd, pointed, boiled* (without salt) {0.11}; Onion, raw {0.11}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.11}</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Chicken leg, without skin, raw {1.05}; UNKNOWN; Green gram, split, boiled* (without salt) {0.33}; Tomato, red, ripe, boiled* (without salt) {0.33}; Cucumber, peeled, raw {0.33}; Onion, raw {0.33}; Radish, boiled* (without salt) {0.33}; Ginger root, raw {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {0.5}; Green gram, split, boiled* (without salt) {0.6}; Tomato, red, ripe, boiled* (without salt) {0.6}; Cucumber, peeled, raw {0.6}; Onion, raw {0.6}; Radish, boiled* (without salt) {0.6}; Ginger root, raw {0.1}</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Hilsha, without bones, raw {0.06}; Hilsha, without bones, raw {0.06}; Chicken leg, without skin, raw {0.06}; UNKNOWN; Green gram, split, boiled* (without salt) {0.16}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.09}; Hilsha, without bones, raw {0.09}; Chicken leg, without skin, raw {1.0}; Green gram, split, boiled* (without salt) {0.33}</t>
         </is>
       </c>
       <c r="AL9" t="inlineStr">
@@ -1964,7 +1964,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.11}; UNKNOWN; Egg, chicken, farmed, boiled* (without salt) {0.17}; Onion, raw {0.11}; Garlic, raw {0.11}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {6.0}; Egg, chicken, farmed, boiled* (without salt) {0.17}; Onion, raw {0.16}; Garlic, raw {0.16}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.11}; UNKNOWN; Hilsha, without bones, raw {0.09}; Rohu, river, raw {0.09}; Green gram, split, boiled* (without salt) {0.11}; Gourd, bitter, boiled* (without salt) {0.11}</t>
+          <t>Rice, BR-28, boiled* (without salt) {4.5}; Hilsha, without bones, raw {0.09}; Rohu, river, raw {0.09}; Green gram, split, boiled* (without salt) {0.16}; Gourd, bitter, boiled* (without salt) {0.16}</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -2026,7 +2026,7 @@
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr">
         <is>
-          <t>Biscuit, sweet* {3.0}; UNKNOWN</t>
+          <t>Biscuit, sweet* {0.9}</t>
         </is>
       </c>
       <c r="X10" t="inlineStr"/>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Hilsha, without bones, raw {0.09}; Rohu, river, raw {0.09}; Green gram, split, boiled* (without salt) {0.16}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Hilsha, without bones, raw {0.09}; Rohu, river, raw {0.09}; Green gram, split, boiled* (without salt) {0.33}</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -2186,7 +2186,7 @@
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.65}; UNKNOWN; Tomato, red, ripe, boiled* (without salt) {0.65}; Goby, Tank goby, raw {1.05}; UNKNOWN; Green gram, split, boiled* (without salt) {0.65}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Tomato, red, ripe, boiled* (without salt) {1.5}; Goby, Tank goby, raw {0.5}; Green gram, split, boiled* (without salt) {1.5}</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.22}; UNKNOWN; Chicken leg, without skin, raw {0.7}; UNKNOWN; Green gram, split, boiled* (without salt) {0.22}; Tomato, red, ripe, boiled* (without salt) {0.22}; Cucumber, peeled, raw {0.22}; Onion, raw {0.22}; Radish, boiled* (without salt) {0.22}; Ginger root, raw {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {1.5}; Green gram, split, boiled* (without salt) {0.4}; Tomato, red, ripe, boiled* (without salt) {0.4}; Cucumber, peeled, raw {0.4}; Onion, raw {0.4}; Radish, boiled* (without salt) {0.4}; Ginger root, raw {0.1}</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -2256,7 +2256,7 @@
       </c>
       <c r="AK11" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.16}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.16}; Onion, raw {0.16}; Chilli, red, dry {0.1}; Prawn, Giant tiger prawn, raw {0.42}; Onion, raw {0.16}; Garlic, raw {0.16}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Potato, Diamond, boiled* (without salt) {0.2}; Onion, raw {0.2}; Chilli, red, dry {0.1}; Prawn, Giant tiger prawn, raw {0.42}; Onion, raw {0.2}; Garlic, raw {0.2}</t>
         </is>
       </c>
       <c r="AL11" t="inlineStr">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Egg, chicken, farmed, boiled* (without salt) {0.35}; UNKNOWN; Garlic, raw {0.33}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.33}; Gourd, ash, raw {0.33}; Prawn, Giant tiger prawn, raw {0.35}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {1.0}; Garlic, raw {0.43}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.43}; Gourd, ash, raw {0.43}; Prawn, Giant tiger prawn, raw {0.7}</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Biscuit, sweet* {0.67}; UNKNOWN; Rice, puffed, salted {0.67}; Onion, raw {0.67}; Soybean oil {0.15}; Chilli, red, dry {0.1}; Lemon, Kagoji, raw {0.1}</t>
+          <t>Biscuit, sweet* {2.0}; Rice, puffed, salted {1.0}; Onion, raw {1.0}; Soybean oil {0.15}; Chilli, red, dry {0.1}; Lemon, Kagoji, raw {0.1}</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr"/>
@@ -2544,10 +2544,14 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.33}; Onion, raw {0.33}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Lotus seeds, dried {0.33}; Spinach, boiled* (without salt) {0.33}; Soybean oil {0.15}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+          <t>Hilsha, without bones, raw {0.7}; Potato, Diamond, boiled* (without salt) {0.26}; Onion, raw {0.26}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Lotus seeds, dried {0.26}; Spinach, boiled* (without salt) {0.26}; Soybean oil {0.15}; Chilli, green, with seeds, raw {0.26}; Coriander seed, dry {0.1}</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Hilsha, without bones, raw</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>Lunch</t>
@@ -2575,7 +2579,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.43}; UNKNOWN; Pangas, without bones, raw {0.7}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.43}; Colocasia/Taro, boiled* (without salt) {0.43}; Salt {0.1}; Soybean oil {0.15}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {2.0}; Potato, Diamond, boiled* (without salt) {1.0}; Colocasia/Taro, boiled* (without salt) {1.0}; Salt {0.1}; Soybean oil {0.15}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -2610,7 +2614,7 @@
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.26}; UNKNOWN; Pumpkin leaves, raw {0.26}; Pangas, without bones, raw {0.7}; Mango, Fazli, orange flesh, ripe, raw {0.26}; Soybean oil {0.15}; Onion, raw {0.26}; Chilli, green, with seeds, raw {0.26}; Coriander seed, dry {0.1}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pumpkin leaves, raw {0.33}; Pangas, without bones, raw {0.7}; Mango, Fazli, orange flesh, ripe, raw {0.33}; Soybean oil {0.15}; Onion, raw {0.33}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
@@ -2641,7 +2645,7 @@
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.97}; UNKNOWN; Pangas, without bones, raw {1.05}; Papaya, unripe, boiled* (without salt) {0.97}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.05}; Papaya, unripe, boiled* (without salt) {1.95}</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
@@ -2692,10 +2696,14 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.33}; Onion, raw {0.33}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Lotus seeds, dried {0.33}; Spinach, boiled* (without salt) {0.33}; Soybean oil {0.15}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
+          <t>Hilsha, without bones, raw {0.7}; Potato, Diamond, boiled* (without salt) {0.26}; Onion, raw {0.26}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Lotus seeds, dried {0.26}; Spinach, boiled* (without salt) {0.26}; Soybean oil {0.15}; Chilli, green, with seeds, raw {0.26}; Coriander seed, dry {0.1}</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Hilsha, without bones, raw</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>Dinner</t>
@@ -2723,7 +2731,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.43}; UNKNOWN; Pangas, without bones, raw {0.7}; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.43}; Colocasia/Taro, boiled* (without salt) {0.43}; Salt {0.1}; Soybean oil {0.15}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {2.0}; Potato, Diamond, boiled* (without salt) {1.0}; Colocasia/Taro, boiled* (without salt) {1.0}; Salt {0.1}; Soybean oil {0.15}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -2785,7 +2793,7 @@
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {1.95}; UNKNOWN; Pangas, without bones, raw {1.05}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {3.0}</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
@@ -2820,14 +2828,10 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Chicken leg, without skin, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.65}; Gourd, pointed, boiled* (without salt) {0.65}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.65}; UNKNOWN</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Chicken leg, without skin, raw</t>
-        </is>
-      </c>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
@@ -2930,7 +2934,7 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {0.33}; UNKNOWN; Pangas, without bones, raw {0.7}; Mango, Fazli, orange flesh, ripe, raw {0.33}; Soybean oil {0.15}; Onion, raw {0.33}; Chilli, green, with seeds, raw {0.33}; Coriander seed, dry {0.1}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {0.7}; Mango, Fazli, orange flesh, ripe, raw {0.43}; Soybean oil {0.15}; Onion, raw {0.43}; Chilli, green, with seeds, raw {0.43}; Coriander seed, dry {0.1}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">

</xml_diff>